<commit_message>
fourth commit done with regards to usage of before and after suite testng
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse 2021 03\Workspace\CTSParabank\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F639C9-E325-440E-ABED-BFB4A48D5885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECB8BF5-E076-430E-A673-85682FF95F1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A52AA3A-C013-419B-921F-5436F3FDD808}"/>
   </bookViews>
@@ -116,7 +116,7 @@
     <t>Debit</t>
   </si>
   <si>
-    <t>1234897</t>
+    <t>1234899</t>
   </si>
 </sst>
 </file>

</xml_diff>